<commit_message>
1 Juta Filament 1 milyar
</commit_message>
<xml_diff>
--- a/public/template.xlsx
+++ b/public/template.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\simoring2\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\proyek\simoring2\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{111B3F7B-72EB-446C-9275-39DF2BB30CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C198351A-E5BA-495B-BA78-D0E71987E8B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{73CE08D0-EAF2-4926-9F6D-563353562EC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>kelas_id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>nis</t>
   </si>
@@ -46,9 +43,6 @@
   </si>
   <si>
     <t>tanggal_lahir</t>
-  </si>
-  <si>
-    <t>angkatan</t>
   </si>
   <si>
     <t>Siswa 31</t>
@@ -410,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4BE3E86-1869-4D94-805C-E2A9C7E489C0}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H2"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -421,7 +415,7 @@
     <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,37 +434,25 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>20240031</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>20240031</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2">
+        <v>8123456789</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2">
-        <v>8123456789</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="1">
+      <c r="F2" s="1">
         <v>39526</v>
-      </c>
-      <c r="H2">
-        <v>2023</v>
       </c>
     </row>
   </sheetData>

</xml_diff>